<commit_message>
Information on 1912 data sources added to metaData tab, additional diseases classified as "neurosyphilis," "Century of death ccb Mapping" excel sheet updated to reflect classification changes made to ccb data for 2019 and 2020 in "Century of death DATA" spreadsheet, "COPD" specific level classification was created (and includes COPD, chronic bronchitis, bronchitis unspecified, and pulmonary emphysema), Respiratory infection in ccb data reclassified as "Influenza/Pneumonia," ccb vs. cdc graphs added back to .rmd file, notes about the excel sorting added to top od .rmd (right below to do list).
</commit_message>
<xml_diff>
--- a/Century of death CCB Mapping.xlsx
+++ b/Century of death CCB Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774C60D7-32CE-BD4A-AD18-E4A78DDB5EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BADCE9-67DD-6042-9F40-B4A490C0AE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="250" r:id="rId4"/>
+    <pivotCache cacheId="17" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="171">
   <si>
     <t>causeCode</t>
   </si>
@@ -542,7 +542,13 @@
     <t>Alzheimer's</t>
   </si>
   <si>
-    <t>Other Neurologic</t>
+    <t>Influenza/Pneumonia</t>
+  </si>
+  <si>
+    <t>Kidney Disease and Diabetes</t>
+  </si>
+  <si>
+    <t>Other Injury</t>
   </si>
 </sst>
 </file>
@@ -572,7 +578,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,12 +607,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -682,12 +682,189 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="35">
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="gray0625">
@@ -1444,7 +1621,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="250" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1934,9 +2111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1998,7 +2175,7 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G2">
@@ -2033,7 +2210,7 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G3">
@@ -2068,7 +2245,7 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G4">
@@ -2103,7 +2280,7 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G5">
@@ -2138,7 +2315,7 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G6">
@@ -2165,15 +2342,15 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>168</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>168</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G7">
@@ -2208,7 +2385,7 @@
       <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G8">
@@ -2243,7 +2420,7 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G9">
@@ -2270,15 +2447,15 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G10">
@@ -2313,7 +2490,7 @@
       <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G11">
@@ -2348,7 +2525,7 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G12">
@@ -2383,7 +2560,7 @@
       <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G13">
@@ -2418,7 +2595,7 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G14">
@@ -2453,7 +2630,7 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G15">
@@ -2488,7 +2665,7 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G16">
@@ -2523,7 +2700,7 @@
       <c r="E17" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G17">
@@ -2558,7 +2735,7 @@
       <c r="E18" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G18">
@@ -2593,7 +2770,7 @@
       <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G19">
@@ -2628,7 +2805,7 @@
       <c r="E20" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G20">
@@ -2663,7 +2840,7 @@
       <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G21">
@@ -2698,7 +2875,7 @@
       <c r="E22" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G22">
@@ -2733,7 +2910,7 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G23">
@@ -2768,7 +2945,7 @@
       <c r="E24" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G24">
@@ -2803,7 +2980,7 @@
       <c r="E25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G25">
@@ -2838,7 +3015,7 @@
       <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G26">
@@ -2873,7 +3050,7 @@
       <c r="E27" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G27">
@@ -2908,7 +3085,7 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G28">
@@ -2943,7 +3120,7 @@
       <c r="E29" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="20" t="s">
         <v>34</v>
       </c>
       <c r="G29">
@@ -2978,7 +3155,7 @@
       <c r="E30" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G30">
@@ -3013,7 +3190,7 @@
       <c r="E31" t="s">
         <v>79</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G31">
@@ -3048,7 +3225,7 @@
       <c r="E32" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G32">
@@ -3083,7 +3260,7 @@
       <c r="E33" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G33">
@@ -3118,7 +3295,7 @@
       <c r="E34" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G34">
@@ -3153,7 +3330,7 @@
       <c r="E35" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G35">
@@ -3180,7 +3357,7 @@
         <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>169</v>
       </c>
       <c r="D36" t="s">
         <v>94</v>
@@ -3188,7 +3365,7 @@
       <c r="E36" t="s">
         <v>95</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G36">
@@ -3223,7 +3400,7 @@
       <c r="E37" t="s">
         <v>95</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G37">
@@ -3258,7 +3435,7 @@
       <c r="E38" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G38">
@@ -3291,9 +3468,9 @@
         <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F39" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G39">
@@ -3319,7 +3496,7 @@
       <c r="B40" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" t="s">
         <v>167</v>
       </c>
       <c r="D40" t="s">
@@ -3328,7 +3505,7 @@
       <c r="E40" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G40">
@@ -3361,9 +3538,9 @@
         <v>102</v>
       </c>
       <c r="E41" t="s">
-        <v>168</v>
-      </c>
-      <c r="F41" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G41">
@@ -3398,7 +3575,7 @@
       <c r="E42" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G42">
@@ -3425,16 +3602,16 @@
         <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="D43" t="s">
         <v>112</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>24</v>
+        <v>95</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="G43">
         <v>2127</v>
@@ -3468,7 +3645,7 @@
       <c r="E44" t="s">
         <v>95</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G44">
@@ -3503,7 +3680,7 @@
       <c r="E45" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="17" t="s">
+      <c r="F45" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G45">
@@ -3529,7 +3706,7 @@
       <c r="B46" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" t="s">
         <v>95</v>
       </c>
       <c r="D46" t="s">
@@ -3538,7 +3715,7 @@
       <c r="E46" t="s">
         <v>124</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G46">
@@ -3564,7 +3741,7 @@
       <c r="B47" t="s">
         <v>121</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" t="s">
         <v>95</v>
       </c>
       <c r="D47" t="s">
@@ -3573,7 +3750,7 @@
       <c r="E47" t="s">
         <v>124</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G47">
@@ -3599,7 +3776,7 @@
       <c r="B48" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" t="s">
         <v>124</v>
       </c>
       <c r="D48" t="s">
@@ -3608,7 +3785,7 @@
       <c r="E48" t="s">
         <v>124</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F48" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G48">
@@ -3643,7 +3820,7 @@
       <c r="E49" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G49">
@@ -3678,7 +3855,7 @@
       <c r="E50" t="s">
         <v>130</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F50" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G50">
@@ -3705,7 +3882,7 @@
         <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D51" t="s">
         <v>130</v>
@@ -3713,7 +3890,7 @@
       <c r="E51" t="s">
         <v>130</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G51">
@@ -3740,7 +3917,7 @@
         <v>134</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D52" t="s">
         <v>130</v>
@@ -3748,7 +3925,7 @@
       <c r="E52" t="s">
         <v>130</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G52">
@@ -3775,7 +3952,7 @@
         <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D53" t="s">
         <v>130</v>
@@ -3783,7 +3960,7 @@
       <c r="E53" t="s">
         <v>130</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G53">
@@ -3810,7 +3987,7 @@
         <v>138</v>
       </c>
       <c r="C54" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
         <v>130</v>
@@ -3818,7 +3995,7 @@
       <c r="E54" t="s">
         <v>130</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G54">
@@ -3853,7 +4030,7 @@
       <c r="E55" t="s">
         <v>130</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G55">
@@ -3888,7 +4065,7 @@
       <c r="E56" t="s">
         <v>130</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G56">
@@ -3915,7 +4092,7 @@
         <v>146</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D57" t="s">
         <v>130</v>
@@ -3923,7 +4100,7 @@
       <c r="E57" t="s">
         <v>130</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F57" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G57">
@@ -3958,7 +4135,7 @@
       <c r="E58" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="17" t="s">
+      <c r="F58" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G58">
@@ -3993,7 +4170,7 @@
       <c r="E59" t="s">
         <v>24</v>
       </c>
-      <c r="F59" s="17" t="s">
+      <c r="F59" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G59">
@@ -4028,7 +4205,7 @@
       <c r="E60" t="s">
         <v>24</v>
       </c>
-      <c r="F60" s="17" t="s">
+      <c r="F60" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G60">
@@ -4055,42 +4232,61 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Cardiovascular">
-      <formula>NOT(ISERROR(SEARCH("Cardiovascular",F2)))</formula>
+  <conditionalFormatting sqref="F61:F1048576">
+    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Cardiovascular">
+      <formula>NOT(ISERROR(SEARCH("Cardiovascular",F61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Injury">
-      <formula>NOT(ISERROR(SEARCH("Injury",F2)))</formula>
+  <conditionalFormatting sqref="F61:F1048576">
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="Injury">
+      <formula>NOT(ISERROR(SEARCH("Injury",F61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Other Chronic">
-      <formula>NOT(ISERROR(SEARCH("Other Chronic",F2)))</formula>
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Other Chronic">
+      <formula>NOT(ISERROR(SEARCH("Other Chronic",F61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Communicable">
-      <formula>NOT(ISERROR(SEARCH("Communicable",F2)))</formula>
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Communicable">
+      <formula>NOT(ISERROR(SEARCH("Communicable",F61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cancer">
-      <formula>NOT(ISERROR(SEARCH("Cancer",F2)))</formula>
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Cancer">
+      <formula>NOT(ISERROR(SEARCH("Cancer",F61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Cardiovascular">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Cardiovascular">
       <formula>NOT(ISERROR(SEARCH("Cardiovascular",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Injury">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="Injury">
       <formula>NOT(ISERROR(SEARCH("Injury",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Other Chronic">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Other Chronic">
       <formula>NOT(ISERROR(SEARCH("Other Chronic",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Communicable">
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Communicable">
       <formula>NOT(ISERROR(SEARCH("Communicable",F1)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Cancer">
+      <formula>NOT(ISERROR(SEARCH("Cancer",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F60">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Cardiovascular">
+      <formula>NOT(ISERROR(SEARCH("Cardiovascular",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F60">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Injury">
+      <formula>NOT(ISERROR(SEARCH("Injury",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Other Chronic">
+      <formula>NOT(ISERROR(SEARCH("Other Chronic",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Communicable">
+      <formula>NOT(ISERROR(SEARCH("Communicable",F2)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Cancer">
-      <formula>NOT(ISERROR(SEARCH("Cancer",F1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Cancer",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed specific level for covid 19 from "Other Communicable" to "COVID-19," specific level for "Other Chronic - Other Respiratory - Other Chronic" was changed to "Chronic Respiratory," population data was added to 1911 and 1912 (though the population for 1912 should be verified, as it had to be calculated from death rates and death numbers), and all changes made to ccb sorting in the "Century of death DATA" file were also applied to the "Century of death CCB Mapping."
</commit_message>
<xml_diff>
--- a/Century of death CCB Mapping.xlsx
+++ b/Century of death CCB Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BADCE9-67DD-6042-9F40-B4A490C0AE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0A783-3CFF-BC4C-B432-D195A09EE32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="173">
   <si>
     <t>causeCode</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>Other Injury</t>
+  </si>
+  <si>
+    <t>Chronic Respiratory</t>
+  </si>
+  <si>
+    <t>COPD</t>
   </si>
 </sst>
 </file>
@@ -689,7 +695,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="gray0625">
@@ -2112,8 +2153,8 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2447,7 +2488,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
@@ -3707,7 +3748,7 @@
         <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
         <v>95</v>
@@ -3742,7 +3783,7 @@
         <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
         <v>95</v>
@@ -4233,40 +4274,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F61:F1048576">
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Cardiovascular">
+    <cfRule type="containsText" dxfId="39" priority="20" operator="containsText" text="Cardiovascular">
       <formula>NOT(ISERROR(SEARCH("Cardiovascular",F61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:F1048576">
-    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="Injury">
+    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="Injury">
       <formula>NOT(ISERROR(SEARCH("Injury",F61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Other Chronic">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Other Chronic">
       <formula>NOT(ISERROR(SEARCH("Other Chronic",F61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Communicable">
+    <cfRule type="containsText" dxfId="36" priority="18" operator="containsText" text="Communicable">
       <formula>NOT(ISERROR(SEARCH("Communicable",F61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Cancer">
+    <cfRule type="containsText" dxfId="35" priority="19" operator="containsText" text="Cancer">
       <formula>NOT(ISERROR(SEARCH("Cancer",F61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Cardiovascular">
+    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Cardiovascular">
       <formula>NOT(ISERROR(SEARCH("Cardiovascular",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="Injury">
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="Injury">
       <formula>NOT(ISERROR(SEARCH("Injury",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Other Chronic">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Other Chronic">
       <formula>NOT(ISERROR(SEARCH("Other Chronic",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Communicable">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Communicable">
       <formula>NOT(ISERROR(SEARCH("Communicable",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Cancer">
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Cancer">
       <formula>NOT(ISERROR(SEARCH("Cancer",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>